<commit_message>
fx chamada: treta nalógica do btt desfazer
</commit_message>
<xml_diff>
--- a/data/relatorioChamada.xlsx
+++ b/data/relatorioChamada.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Lista 2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Lista-de-Chamada-Web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22AEF58-378C-407F-A967-A4C4920E5CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA3EFFF-48BE-48AE-BD84-277D6F1B3482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E062E1E0-D6DA-4B03-B8FF-70AA7DD5E231}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <cols>
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="14" width="3.5703125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
app web 1.0 90% - falta integar
</commit_message>
<xml_diff>
--- a/data/relatorioChamada.xlsx
+++ b/data/relatorioChamada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Lista-de-Chamada-Web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA3EFFF-48BE-48AE-BD84-277D6F1B3482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2508F0E9-A147-47F6-B2C4-4211E442695B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E062E1E0-D6DA-4B03-B8FF-70AA7DD5E231}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="11070" xr2:uid="{E062E1E0-D6DA-4B03-B8FF-70AA7DD5E231}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>parQ</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Aniversário</t>
+  </si>
+  <si>
+    <t>nível:</t>
+  </si>
+  <si>
+    <t>Observações</t>
   </si>
 </sst>
 </file>
@@ -466,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4F9505-5707-422A-88FD-F3D678E847CD}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,9 +485,10 @@
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="14" width="3.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -492,7 +499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -503,17 +510,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -521,7 +531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -544,6 +554,9 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>